<commit_message>
Update Các bước chuyển đổi
</commit_message>
<xml_diff>
--- a/PG/Tai_Lieu_(VN)/Thông tin chung - CONTEC.xlsx
+++ b/PG/Tai_Lieu_(VN)/Thông tin chung - CONTEC.xlsx
@@ -5,19 +5,19 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thach\Desktop\CONTEC_Migration\PG\Tai_Lieu_(VN)\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20325" windowHeight="7080"/>
   </bookViews>
   <sheets>
-    <sheet name="setup môi trường" sheetId="4" r:id="rId1"/>
-    <sheet name="Tk login vào máy Remote" sheetId="1" r:id="rId2"/>
-    <sheet name="các bước chuyển đổi" sheetId="2" r:id="rId3"/>
-    <sheet name="thông tin kết nối DB" sheetId="3" r:id="rId4"/>
+    <sheet name="Các bước chuyển đổi" sheetId="2" r:id="rId1"/>
+    <sheet name="Setup môi trường" sheetId="4" r:id="rId2"/>
+    <sheet name="Tk login vào máy Remote" sheetId="1" r:id="rId3"/>
+    <sheet name="Thông tin kết nối DB" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
   <si>
     <t>cis07@ad.fjazure.com</t>
   </si>
@@ -117,9 +117,6 @@
   </si>
   <si>
     <t>3/ "CLTIDCONTEC  "</t>
-  </si>
-  <si>
-    <t>8/ Build hết lỗi và F5 Run chạy được màn hình  --&gt;   (Tiến độ là 50%)</t>
   </si>
   <si>
     <t>9/ Bấm từng nút ở phía trên F1-F12 và fix lỗi (tham khảo source mẫu)</t>
@@ -253,12 +250,18 @@
   <si>
     <t>⑬ hoàn thành kết nối remote</t>
   </si>
+  <si>
+    <t>4/ Copy file "SSSWIN.INI" trong  E:\CRAFT\PG\共通ini   vào thư mục bin của Project mình !</t>
+  </si>
+  <si>
+    <t>8/ Build hết lỗi và F5 Run chạy được màn hình  --&gt;   (Tiến độ là 30%)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -270,6 +273,29 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -296,12 +322,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2503,9 +2532,154 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:B35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="4"/>
+    </row>
+    <row r="5" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="4"/>
+    </row>
+    <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="4"/>
+    </row>
+    <row r="9" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="4"/>
+    </row>
+    <row r="11" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="4"/>
+    </row>
+    <row r="13" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B13" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B14" s="4"/>
+    </row>
+    <row r="15" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B15" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B16" s="4"/>
+    </row>
+    <row r="17" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B17" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B18" s="4"/>
+    </row>
+    <row r="19" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B19" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B20" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B21" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B22" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B23" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B24" s="4"/>
+    </row>
+    <row r="25" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B25" s="4"/>
+    </row>
+    <row r="26" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B26" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B27" s="4"/>
+    </row>
+    <row r="28" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B28" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B29" s="4"/>
+    </row>
+    <row r="30" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B30" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B31" s="4"/>
+    </row>
+    <row r="32" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B32" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B35" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:S491"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A151" workbookViewId="0">
       <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
@@ -2513,7 +2687,7 @@
   <sheetData>
     <row r="2" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -3115,7 +3289,7 @@
     </row>
     <row r="32" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
@@ -3697,7 +3871,7 @@
     </row>
     <row r="61" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B61" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
@@ -4219,7 +4393,7 @@
     </row>
     <row r="87" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B87" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C87" s="1"/>
       <c r="D87" s="1"/>
@@ -4821,7 +4995,7 @@
     </row>
     <row r="117" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B117" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C117" s="1"/>
       <c r="D117" s="1"/>
@@ -5523,7 +5697,7 @@
     </row>
     <row r="152" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B152" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C152" s="1"/>
       <c r="D152" s="1"/>
@@ -5945,10 +6119,10 @@
     </row>
     <row r="173" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B173" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D173" s="1"/>
       <c r="E173" s="1"/>
@@ -5970,7 +6144,7 @@
     <row r="174" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B174" s="1"/>
       <c r="C174" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D174" s="1"/>
       <c r="E174" s="1"/>
@@ -5992,7 +6166,7 @@
     <row r="175" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B175" s="1"/>
       <c r="C175" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D175" s="1"/>
       <c r="E175" s="1"/>
@@ -6014,7 +6188,7 @@
     <row r="176" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B176" s="1"/>
       <c r="C176" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D176" s="1"/>
       <c r="E176" s="1"/>
@@ -6435,7 +6609,7 @@
     </row>
     <row r="197" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B197" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C197" s="1"/>
       <c r="D197" s="1"/>
@@ -6857,7 +7031,7 @@
     </row>
     <row r="218" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B218" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C218" s="1"/>
       <c r="D218" s="1"/>
@@ -7459,7 +7633,7 @@
     </row>
     <row r="248" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B248" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C248" s="1"/>
       <c r="D248" s="1"/>
@@ -7481,7 +7655,7 @@
     </row>
     <row r="249" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B249" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C249" s="1"/>
       <c r="D249" s="1"/>
@@ -7883,7 +8057,7 @@
     </row>
     <row r="269" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B269" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C269" s="1"/>
       <c r="D269" s="1"/>
@@ -8465,7 +8639,7 @@
     </row>
     <row r="298" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B298" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C298" s="1"/>
       <c r="D298" s="1"/>
@@ -9067,7 +9241,7 @@
     </row>
     <row r="328" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B328" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C328" s="1"/>
       <c r="D328" s="1"/>
@@ -9629,7 +9803,7 @@
     </row>
     <row r="356" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B356" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C356" s="1"/>
       <c r="D356" s="1"/>
@@ -9651,7 +9825,7 @@
     </row>
     <row r="357" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B357" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C357" s="1"/>
       <c r="D357" s="1"/>
@@ -9673,7 +9847,7 @@
     </row>
     <row r="358" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B358" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C358" s="1"/>
       <c r="D358" s="1"/>
@@ -9735,7 +9909,7 @@
     </row>
     <row r="361" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B361" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C361" s="1"/>
       <c r="D361" s="1"/>
@@ -12361,18 +12535,18 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="3" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="G3" t="s">
@@ -12452,107 +12626,8 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C18" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:B33"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
-        <v>34</v>
-      </c>
-    </row>
-  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -12562,24 +12637,24 @@
   <dimension ref="B3:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>36</v>
-      </c>
-    </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>